<commit_message>
-updating fuel supply and steel plant data
</commit_message>
<xml_diff>
--- a/inst/extdata/fuel supply.xlsx
+++ b/inst/extdata/fuel supply.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Documents\RPackages\china_co2\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\CREA-China\monthly snapshot\wind data templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FADA31B-7C3A-42B3-A996-21E19B4F8A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F68D027-F30B-4949-8746-D35B027E16A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25890" windowHeight="15690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Output_Natural Crude Oil_YTD" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -173,40 +173,34 @@
     <t>Update</t>
   </si>
   <si>
-    <t>1989-02:2023-09</t>
-  </si>
-  <si>
-    <t>1995-01:2023-09</t>
-  </si>
-  <si>
-    <t>1989-01:2023-09</t>
-  </si>
-  <si>
-    <t>2023-10-18</t>
-  </si>
-  <si>
     <t>1989-02:2023-10</t>
   </si>
   <si>
     <t>1995-01:2023-10</t>
   </si>
   <si>
-    <t>2003-07:2023-10</t>
+    <t>1989-02:2023-11</t>
   </si>
   <si>
-    <t>1989-01:2023-10</t>
+    <t>1995-01:2023-11</t>
   </si>
   <si>
-    <t>2023-11-15</t>
+    <t>2003-07:2023-11</t>
   </si>
   <si>
-    <t>2023-11-07</t>
+    <t>1989-01:2023-11</t>
   </si>
   <si>
-    <t>2023-10-23</t>
+    <t>2023-12-15</t>
   </si>
   <si>
-    <t>2023-10-19</t>
+    <t>2023-12-07</t>
+  </si>
+  <si>
+    <t>2023-11-27</t>
+  </si>
+  <si>
+    <t>2023-11-16</t>
   </si>
 </sst>
 </file>
@@ -217,7 +211,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm"/>
     <numFmt numFmtId="165" formatCode="#,##0.00_ "/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    <numFmt numFmtId="171" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.000000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -273,19 +267,19 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,20 +620,20 @@
   <dimension ref="A1:P430"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B402" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B412" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="B2" sqref="B2"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="F412" sqref="F412"/>
+      <selection pane="bottomRight" activeCell="A403" sqref="A403"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -648,291 +642,291 @@
         <v>Wind</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="174">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="1:14" ht="195">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="E6" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="H6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="C8" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="4" t="s">
+      <c r="H8" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="K8" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="L8" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="M8" s="10" t="s">
         <v>47</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -975,7 +969,7 @@
       <c r="M9" s="3">
         <v>0</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="5">
         <f t="shared" ref="N9:N72" si="0">E9-D9</f>
         <v>0</v>
       </c>
@@ -1020,7 +1014,7 @@
       <c r="M10" s="3">
         <v>64.8</v>
       </c>
-      <c r="N10" s="8">
+      <c r="N10" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1065,7 +1059,7 @@
       <c r="M11" s="3">
         <v>100.8</v>
       </c>
-      <c r="N11" s="8">
+      <c r="N11" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1110,7 +1104,7 @@
       <c r="M12" s="3">
         <v>132.6</v>
       </c>
-      <c r="N12" s="8">
+      <c r="N12" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1155,7 +1149,7 @@
       <c r="M13" s="3">
         <v>164.5</v>
       </c>
-      <c r="N13" s="8">
+      <c r="N13" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1200,7 +1194,7 @@
       <c r="M14" s="3">
         <v>198.1</v>
       </c>
-      <c r="N14" s="8">
+      <c r="N14" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1245,7 +1239,7 @@
       <c r="M15" s="3">
         <v>232.3</v>
       </c>
-      <c r="N15" s="8">
+      <c r="N15" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1290,7 +1284,7 @@
       <c r="M16" s="3">
         <v>269.2</v>
       </c>
-      <c r="N16" s="8">
+      <c r="N16" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1335,7 +1329,7 @@
       <c r="M17" s="3">
         <v>300.60000000000002</v>
       </c>
-      <c r="N17" s="8">
+      <c r="N17" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1380,7 +1374,7 @@
       <c r="M18" s="3">
         <v>333.9</v>
       </c>
-      <c r="N18" s="8">
+      <c r="N18" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1425,7 +1419,7 @@
       <c r="M19" s="3">
         <v>368.3</v>
       </c>
-      <c r="N19" s="8">
+      <c r="N19" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1470,7 +1464,7 @@
       <c r="M20" s="3">
         <v>395.2</v>
       </c>
-      <c r="N20" s="8">
+      <c r="N20" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1515,7 +1509,7 @@
       <c r="M21" s="3">
         <v>31</v>
       </c>
-      <c r="N21" s="8">
+      <c r="N21" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1560,7 +1554,7 @@
       <c r="M22" s="3">
         <v>56.6</v>
       </c>
-      <c r="N22" s="8">
+      <c r="N22" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1605,7 +1599,7 @@
       <c r="M23" s="3">
         <v>92.2</v>
       </c>
-      <c r="N23" s="8">
+      <c r="N23" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1650,7 +1644,7 @@
       <c r="M24" s="3">
         <v>128.69999999999999</v>
       </c>
-      <c r="N24" s="8">
+      <c r="N24" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1695,7 +1689,7 @@
       <c r="M25" s="3">
         <v>168</v>
       </c>
-      <c r="N25" s="8">
+      <c r="N25" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1740,7 +1734,7 @@
       <c r="M26" s="3">
         <v>202.8</v>
       </c>
-      <c r="N26" s="8">
+      <c r="N26" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1785,7 +1779,7 @@
       <c r="M27" s="3">
         <v>242.2</v>
       </c>
-      <c r="N27" s="8">
+      <c r="N27" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1830,7 +1824,7 @@
       <c r="M28" s="3">
         <v>276.5</v>
       </c>
-      <c r="N28" s="8">
+      <c r="N28" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1875,7 +1869,7 @@
       <c r="M29" s="3">
         <v>306.2</v>
       </c>
-      <c r="N29" s="8">
+      <c r="N29" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1920,7 +1914,7 @@
       <c r="M30" s="3">
         <v>336.3</v>
       </c>
-      <c r="N30" s="8">
+      <c r="N30" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1965,7 +1959,7 @@
       <c r="M31" s="3">
         <v>362.2</v>
       </c>
-      <c r="N31" s="8">
+      <c r="N31" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2010,7 +2004,7 @@
       <c r="M32" s="3">
         <v>384.5</v>
       </c>
-      <c r="N32" s="8">
+      <c r="N32" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2055,7 +2049,7 @@
       <c r="M33" s="3">
         <v>32.6</v>
       </c>
-      <c r="N33" s="8">
+      <c r="N33" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2100,7 +2094,7 @@
       <c r="M34" s="3">
         <v>61.1</v>
       </c>
-      <c r="N34" s="8">
+      <c r="N34" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2145,7 +2139,7 @@
       <c r="M35" s="3">
         <v>96.2</v>
       </c>
-      <c r="N35" s="8">
+      <c r="N35" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2190,7 +2184,7 @@
       <c r="M36" s="3">
         <v>126.4</v>
       </c>
-      <c r="N36" s="8">
+      <c r="N36" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2235,7 +2229,7 @@
       <c r="M37" s="3">
         <v>158.80000000000001</v>
       </c>
-      <c r="N37" s="8">
+      <c r="N37" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2280,7 +2274,7 @@
       <c r="M38" s="3">
         <v>196</v>
       </c>
-      <c r="N38" s="8">
+      <c r="N38" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2325,7 +2319,7 @@
       <c r="M39" s="3">
         <v>231.8</v>
       </c>
-      <c r="N39" s="8">
+      <c r="N39" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2370,7 +2364,7 @@
       <c r="M40" s="3">
         <v>267.60000000000002</v>
       </c>
-      <c r="N40" s="8">
+      <c r="N40" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2415,7 +2409,7 @@
       <c r="M41" s="3">
         <v>301.5</v>
       </c>
-      <c r="N41" s="8">
+      <c r="N41" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2460,7 +2454,7 @@
       <c r="M42" s="3">
         <v>339.4</v>
       </c>
-      <c r="N42" s="8">
+      <c r="N42" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2505,7 +2499,7 @@
       <c r="M43" s="3">
         <v>375.1</v>
       </c>
-      <c r="N43" s="8">
+      <c r="N43" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2550,7 +2544,7 @@
       <c r="M44" s="3">
         <v>398.41</v>
       </c>
-      <c r="N44" s="8">
+      <c r="N44" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2595,7 +2589,7 @@
       <c r="M45" s="3">
         <v>28.2</v>
       </c>
-      <c r="N45" s="8">
+      <c r="N45" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2640,7 +2634,7 @@
       <c r="M46" s="3">
         <v>62.8</v>
       </c>
-      <c r="N46" s="8">
+      <c r="N46" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2685,7 +2679,7 @@
       <c r="M47" s="3">
         <v>99.5</v>
       </c>
-      <c r="N47" s="8">
+      <c r="N47" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2730,7 +2724,7 @@
       <c r="M48" s="3">
         <v>147.5</v>
       </c>
-      <c r="N48" s="8">
+      <c r="N48" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2775,7 +2769,7 @@
       <c r="M49" s="3">
         <v>177.8</v>
       </c>
-      <c r="N49" s="8">
+      <c r="N49" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2820,7 +2814,7 @@
       <c r="M50" s="3">
         <v>209.5</v>
       </c>
-      <c r="N50" s="8">
+      <c r="N50" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2865,7 +2859,7 @@
       <c r="M51" s="3">
         <v>243.2</v>
       </c>
-      <c r="N51" s="8">
+      <c r="N51" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2910,7 +2904,7 @@
       <c r="M52" s="3">
         <v>279.5</v>
       </c>
-      <c r="N52" s="8">
+      <c r="N52" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2955,7 +2949,7 @@
       <c r="M53" s="3">
         <v>310</v>
       </c>
-      <c r="N53" s="8">
+      <c r="N53" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3000,7 +2994,7 @@
       <c r="M54" s="3">
         <v>341.5</v>
       </c>
-      <c r="N54" s="8">
+      <c r="N54" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3045,7 +3039,7 @@
       <c r="M55" s="3">
         <v>371.5</v>
       </c>
-      <c r="N55" s="8">
+      <c r="N55" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3090,7 +3084,7 @@
       <c r="M56" s="3">
         <v>395.9</v>
       </c>
-      <c r="N56" s="8">
+      <c r="N56" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3135,7 +3129,7 @@
       <c r="M57" s="3">
         <v>32</v>
       </c>
-      <c r="N57" s="8">
+      <c r="N57" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3180,7 +3174,7 @@
       <c r="M58" s="3">
         <v>59.6</v>
       </c>
-      <c r="N58" s="8">
+      <c r="N58" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3225,7 +3219,7 @@
       <c r="M59" s="3">
         <v>89.3</v>
       </c>
-      <c r="N59" s="8">
+      <c r="N59" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3270,7 +3264,7 @@
       <c r="M60" s="3">
         <v>117.4</v>
       </c>
-      <c r="N60" s="8">
+      <c r="N60" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3315,7 +3309,7 @@
       <c r="M61" s="3">
         <v>151.1</v>
       </c>
-      <c r="N61" s="8">
+      <c r="N61" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3360,7 +3354,7 @@
       <c r="M62" s="3">
         <v>181.8</v>
       </c>
-      <c r="N62" s="8">
+      <c r="N62" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3405,7 +3399,7 @@
       <c r="M63" s="3">
         <v>214.5</v>
       </c>
-      <c r="N63" s="8">
+      <c r="N63" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3450,7 +3444,7 @@
       <c r="M64" s="3">
         <v>244.8</v>
       </c>
-      <c r="N64" s="8">
+      <c r="N64" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3495,7 +3489,7 @@
       <c r="M65" s="3">
         <v>274.2</v>
       </c>
-      <c r="N65" s="8">
+      <c r="N65" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3540,7 +3534,7 @@
       <c r="M66" s="3">
         <v>308.89999999999998</v>
       </c>
-      <c r="N66" s="8">
+      <c r="N66" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3585,7 +3579,7 @@
       <c r="M67" s="3">
         <v>343.6</v>
       </c>
-      <c r="N67" s="8">
+      <c r="N67" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3630,7 +3624,7 @@
       <c r="M68" s="3">
         <v>373.3</v>
       </c>
-      <c r="N68" s="8">
+      <c r="N68" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3675,7 +3669,7 @@
       <c r="M69" s="3">
         <v>34.4</v>
       </c>
-      <c r="N69" s="8">
+      <c r="N69" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3720,7 +3714,7 @@
       <c r="M70" s="3">
         <v>71.89</v>
       </c>
-      <c r="N70" s="8">
+      <c r="N70" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3765,7 +3759,7 @@
       <c r="M71" s="3">
         <v>115.41</v>
       </c>
-      <c r="N71" s="8">
+      <c r="N71" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3810,7 +3804,7 @@
       <c r="M72" s="3">
         <v>153.88999999999999</v>
       </c>
-      <c r="N72" s="8">
+      <c r="N72" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3855,7 +3849,7 @@
       <c r="M73" s="3">
         <v>190.93</v>
       </c>
-      <c r="N73" s="8">
+      <c r="N73" s="5">
         <f t="shared" ref="N73:N136" si="1">E73-D73</f>
         <v>0</v>
       </c>
@@ -3900,7 +3894,7 @@
       <c r="M74" s="3">
         <v>228.5</v>
       </c>
-      <c r="N74" s="8">
+      <c r="N74" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3945,7 +3939,7 @@
       <c r="M75" s="3">
         <v>267.49</v>
       </c>
-      <c r="N75" s="8">
+      <c r="N75" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3990,7 +3984,7 @@
       <c r="M76" s="3">
         <v>305.77</v>
       </c>
-      <c r="N76" s="8">
+      <c r="N76" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4035,7 +4029,7 @@
       <c r="M77" s="3">
         <v>334.77</v>
       </c>
-      <c r="N77" s="8">
+      <c r="N77" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4080,7 +4074,7 @@
       <c r="M78" s="3">
         <v>368.17</v>
       </c>
-      <c r="N78" s="8">
+      <c r="N78" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4125,7 +4119,7 @@
       <c r="M79" s="3">
         <v>400.64</v>
       </c>
-      <c r="N79" s="8">
+      <c r="N79" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4170,7 +4164,7 @@
       <c r="M80" s="3">
         <v>433.42</v>
       </c>
-      <c r="N80" s="8">
+      <c r="N80" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4215,7 +4209,7 @@
       <c r="M81" s="3">
         <v>35.24</v>
       </c>
-      <c r="N81" s="8">
+      <c r="N81" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4260,7 +4254,7 @@
       <c r="M82" s="3">
         <v>66.83</v>
       </c>
-      <c r="N82" s="8">
+      <c r="N82" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4305,7 +4299,7 @@
       <c r="M83" s="3">
         <v>98.49</v>
       </c>
-      <c r="N83" s="8">
+      <c r="N83" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4350,7 +4344,7 @@
       <c r="M84" s="3">
         <v>131.31</v>
       </c>
-      <c r="N84" s="8">
+      <c r="N84" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4395,7 +4389,7 @@
       <c r="M85" s="3">
         <v>166.7</v>
       </c>
-      <c r="N85" s="8">
+      <c r="N85" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4440,7 +4434,7 @@
       <c r="M86" s="3">
         <v>201.44</v>
       </c>
-      <c r="N86" s="8">
+      <c r="N86" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4485,7 +4479,7 @@
       <c r="M87" s="3">
         <v>239.13</v>
       </c>
-      <c r="N87" s="8">
+      <c r="N87" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4530,7 +4524,7 @@
       <c r="M88" s="3">
         <v>279.62</v>
       </c>
-      <c r="N88" s="8">
+      <c r="N88" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4575,7 +4569,7 @@
       <c r="M89" s="3">
         <v>318.99</v>
       </c>
-      <c r="N89" s="8">
+      <c r="N89" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4620,7 +4614,7 @@
       <c r="M90" s="3">
         <v>357.96</v>
       </c>
-      <c r="N90" s="8">
+      <c r="N90" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4665,7 +4659,7 @@
       <c r="M91" s="3">
         <v>398.71</v>
       </c>
-      <c r="N91" s="8">
+      <c r="N91" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4710,7 +4704,7 @@
       <c r="M92" s="3">
         <v>435.32</v>
       </c>
-      <c r="N92" s="8">
+      <c r="N92" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4755,7 +4749,7 @@
       <c r="M93" s="3">
         <v>37.39</v>
       </c>
-      <c r="N93" s="8">
+      <c r="N93" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4800,7 +4794,7 @@
       <c r="M94" s="3">
         <v>77.87</v>
       </c>
-      <c r="N94" s="8">
+      <c r="N94" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4845,7 +4839,7 @@
       <c r="M95" s="3">
         <v>116.65</v>
       </c>
-      <c r="N95" s="8">
+      <c r="N95" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4890,7 +4884,7 @@
       <c r="M96" s="3">
         <v>158.09</v>
       </c>
-      <c r="N96" s="8">
+      <c r="N96" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4935,7 +4929,7 @@
       <c r="M97" s="3">
         <v>207.18</v>
       </c>
-      <c r="N97" s="8">
+      <c r="N97" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4980,7 +4974,7 @@
       <c r="M98" s="3">
         <v>257.3</v>
       </c>
-      <c r="N98" s="8">
+      <c r="N98" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5025,7 +5019,7 @@
       <c r="M99" s="3">
         <v>297.32</v>
       </c>
-      <c r="N99" s="8">
+      <c r="N99" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5070,7 +5064,7 @@
       <c r="M100" s="3">
         <v>343.02</v>
       </c>
-      <c r="N100" s="8">
+      <c r="N100" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5115,7 +5109,7 @@
       <c r="M101" s="3">
         <v>388.04</v>
       </c>
-      <c r="N101" s="8">
+      <c r="N101" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5160,7 +5154,7 @@
       <c r="M102" s="3">
         <v>436.75</v>
       </c>
-      <c r="N102" s="8">
+      <c r="N102" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5205,7 +5199,7 @@
       <c r="M103" s="3">
         <v>482.99</v>
       </c>
-      <c r="N103" s="8">
+      <c r="N103" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5250,7 +5244,7 @@
       <c r="M104" s="3">
         <v>529.17999999999995</v>
       </c>
-      <c r="N104" s="8">
+      <c r="N104" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5295,7 +5289,7 @@
       <c r="M105" s="3">
         <v>42.33</v>
       </c>
-      <c r="N105" s="8">
+      <c r="N105" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5340,7 +5334,7 @@
       <c r="M106" s="3">
         <v>102.04</v>
       </c>
-      <c r="N106" s="8">
+      <c r="N106" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5385,7 +5379,7 @@
       <c r="M107" s="3">
         <v>126.12</v>
       </c>
-      <c r="N107" s="8">
+      <c r="N107" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5430,7 +5424,7 @@
       <c r="M108" s="3">
         <v>171.34</v>
       </c>
-      <c r="N108" s="8">
+      <c r="N108" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5475,7 +5469,7 @@
       <c r="M109" s="3">
         <v>217.64</v>
       </c>
-      <c r="N109" s="8">
+      <c r="N109" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5520,7 +5514,7 @@
       <c r="M110" s="3">
         <v>265.24</v>
       </c>
-      <c r="N110" s="8">
+      <c r="N110" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5565,7 +5559,7 @@
       <c r="M111" s="3">
         <v>310.98</v>
       </c>
-      <c r="N111" s="8">
+      <c r="N111" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5610,7 +5604,7 @@
       <c r="M112" s="3">
         <v>361.3</v>
       </c>
-      <c r="N112" s="8">
+      <c r="N112" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5655,7 +5649,7 @@
       <c r="M113" s="3">
         <v>415.32</v>
       </c>
-      <c r="N113" s="8">
+      <c r="N113" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5700,7 +5694,7 @@
       <c r="M114" s="3">
         <v>472.1</v>
       </c>
-      <c r="N114" s="8">
+      <c r="N114" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5745,7 +5739,7 @@
       <c r="M115" s="3">
         <v>523.80999999999995</v>
       </c>
-      <c r="N115" s="8">
+      <c r="N115" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5790,7 +5784,7 @@
       <c r="M116" s="3">
         <v>573.69000000000005</v>
       </c>
-      <c r="N116" s="8">
+      <c r="N116" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5835,7 +5829,7 @@
       <c r="M117" s="3">
         <v>48.25</v>
       </c>
-      <c r="N117" s="8">
+      <c r="N117" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5880,7 +5874,7 @@
       <c r="M118" s="3">
         <v>99.69</v>
       </c>
-      <c r="N118" s="8">
+      <c r="N118" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5925,7 +5919,7 @@
       <c r="M119" s="3">
         <v>154.71</v>
       </c>
-      <c r="N119" s="8">
+      <c r="N119" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5970,7 +5964,7 @@
       <c r="M120" s="3">
         <v>206.84</v>
       </c>
-      <c r="N120" s="8">
+      <c r="N120" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6015,7 +6009,7 @@
       <c r="M121" s="3">
         <v>260.62</v>
       </c>
-      <c r="N121" s="8">
+      <c r="N121" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6060,7 +6054,7 @@
       <c r="M122" s="3">
         <v>311.55</v>
       </c>
-      <c r="N122" s="8">
+      <c r="N122" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6105,7 +6099,7 @@
       <c r="M123" s="3">
         <v>359.08</v>
       </c>
-      <c r="N123" s="8">
+      <c r="N123" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6150,7 +6144,7 @@
       <c r="M124" s="3">
         <v>406.54</v>
       </c>
-      <c r="N124" s="8">
+      <c r="N124" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6195,7 +6189,7 @@
       <c r="M125" s="3">
         <v>456.86</v>
       </c>
-      <c r="N125" s="8">
+      <c r="N125" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6240,7 +6234,7 @@
       <c r="M126" s="3">
         <v>511.41</v>
       </c>
-      <c r="N126" s="8">
+      <c r="N126" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6285,7 +6279,7 @@
       <c r="M127" s="3">
         <v>567.95000000000005</v>
       </c>
-      <c r="N127" s="8">
+      <c r="N127" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6330,7 +6324,7 @@
       <c r="M128" s="3">
         <v>574.89</v>
       </c>
-      <c r="N128" s="8">
+      <c r="N128" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6375,7 +6369,7 @@
       <c r="M129" s="3">
         <v>43.3</v>
       </c>
-      <c r="N129" s="8">
+      <c r="N129" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6420,7 +6414,7 @@
       <c r="M130" s="3">
         <v>95.9</v>
       </c>
-      <c r="N130" s="8">
+      <c r="N130" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6465,7 +6459,7 @@
       <c r="M131" s="3">
         <v>147.26</v>
       </c>
-      <c r="N131" s="8">
+      <c r="N131" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6510,7 +6504,7 @@
       <c r="M132" s="3">
         <v>208.29</v>
       </c>
-      <c r="N132" s="8">
+      <c r="N132" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6555,7 +6549,7 @@
       <c r="M133" s="3">
         <v>262.04000000000002</v>
       </c>
-      <c r="N133" s="8">
+      <c r="N133" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6600,7 +6594,7 @@
       <c r="M134" s="3">
         <v>326.48</v>
       </c>
-      <c r="N134" s="8">
+      <c r="N134" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6645,7 +6639,7 @@
       <c r="M135" s="3">
         <v>390.93</v>
       </c>
-      <c r="N135" s="8">
+      <c r="N135" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6690,7 +6684,7 @@
       <c r="M136" s="3">
         <v>461.82</v>
       </c>
-      <c r="N136" s="8">
+      <c r="N136" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6735,7 +6729,7 @@
       <c r="M137" s="3">
         <v>529.01</v>
       </c>
-      <c r="N137" s="8">
+      <c r="N137" s="5">
         <f t="shared" ref="N137:N200" si="2">E137-D137</f>
         <v>0</v>
       </c>
@@ -6780,7 +6774,7 @@
       <c r="M138" s="3">
         <v>606.17999999999995</v>
       </c>
-      <c r="N138" s="8">
+      <c r="N138" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -6825,7 +6819,7 @@
       <c r="M139" s="3">
         <v>670.21</v>
       </c>
-      <c r="N139" s="8">
+      <c r="N139" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -6870,7 +6864,7 @@
       <c r="M140" s="3">
         <v>719.46</v>
       </c>
-      <c r="N140" s="8">
+      <c r="N140" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -6915,7 +6909,7 @@
       <c r="M141" s="3">
         <v>52.55</v>
       </c>
-      <c r="N141" s="8">
+      <c r="N141" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -6960,7 +6954,7 @@
       <c r="M142" s="3">
         <v>113.48</v>
       </c>
-      <c r="N142" s="8">
+      <c r="N142" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7005,7 +6999,7 @@
       <c r="M143" s="3">
         <v>205.46</v>
       </c>
-      <c r="N143" s="8">
+      <c r="N143" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7050,7 +7044,7 @@
       <c r="M144" s="3">
         <v>283.3</v>
       </c>
-      <c r="N144" s="8">
+      <c r="N144" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7095,7 +7089,7 @@
       <c r="M145" s="3">
         <v>358.82</v>
       </c>
-      <c r="N145" s="8">
+      <c r="N145" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7140,7 +7134,7 @@
       <c r="M146" s="3">
         <v>437.63</v>
       </c>
-      <c r="N146" s="8">
+      <c r="N146" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7185,7 +7179,7 @@
       <c r="M147" s="3">
         <v>511.06</v>
       </c>
-      <c r="N147" s="8">
+      <c r="N147" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7230,7 +7224,7 @@
       <c r="M148" s="3">
         <v>583.04999999999995</v>
       </c>
-      <c r="N148" s="8">
+      <c r="N148" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7275,7 +7269,7 @@
       <c r="M149" s="3">
         <v>655.44</v>
       </c>
-      <c r="N149" s="8">
+      <c r="N149" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7320,7 +7314,7 @@
       <c r="M150" s="3">
         <v>727.93</v>
       </c>
-      <c r="N150" s="8">
+      <c r="N150" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7365,7 +7359,7 @@
       <c r="M151" s="3">
         <v>800.24</v>
       </c>
-      <c r="N151" s="8">
+      <c r="N151" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7410,7 +7404,7 @@
       <c r="M152" s="3">
         <v>872.29</v>
       </c>
-      <c r="N152" s="8">
+      <c r="N152" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7455,7 +7449,7 @@
       <c r="M153" s="3">
         <v>61.52</v>
       </c>
-      <c r="N153" s="8">
+      <c r="N153" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7500,7 +7494,7 @@
       <c r="M154" s="3">
         <v>120.01</v>
       </c>
-      <c r="N154" s="8">
+      <c r="N154" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7545,7 +7539,7 @@
       <c r="M155" s="3">
         <v>182.29</v>
       </c>
-      <c r="N155" s="8">
+      <c r="N155" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7590,7 +7584,7 @@
       <c r="M156" s="3">
         <v>244.62</v>
       </c>
-      <c r="N156" s="8">
+      <c r="N156" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7635,7 +7629,7 @@
       <c r="M157" s="3">
         <v>316.52</v>
       </c>
-      <c r="N157" s="8">
+      <c r="N157" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7680,7 +7674,7 @@
       <c r="M158" s="3">
         <v>389.45</v>
       </c>
-      <c r="N158" s="8">
+      <c r="N158" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7725,7 +7719,7 @@
       <c r="M159" s="3">
         <v>458.77</v>
       </c>
-      <c r="N159" s="8">
+      <c r="N159" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7770,7 +7764,7 @@
       <c r="M160" s="3">
         <v>526.63</v>
       </c>
-      <c r="N160" s="8">
+      <c r="N160" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7815,7 +7809,7 @@
       <c r="M161" s="3">
         <v>590.41</v>
       </c>
-      <c r="N161" s="8">
+      <c r="N161" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7860,7 +7854,7 @@
       <c r="M162" s="3">
         <v>662.82</v>
       </c>
-      <c r="N162" s="8">
+      <c r="N162" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7905,7 +7899,7 @@
       <c r="M163" s="3">
         <v>733.46</v>
       </c>
-      <c r="N163" s="8">
+      <c r="N163" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7950,7 +7944,7 @@
       <c r="M164" s="3">
         <v>789.35</v>
       </c>
-      <c r="N164" s="8">
+      <c r="N164" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -7995,7 +7989,7 @@
       <c r="M165" s="3">
         <v>55.38</v>
       </c>
-      <c r="N165" s="8">
+      <c r="N165" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8040,7 +8034,7 @@
       <c r="M166" s="3">
         <v>117.58</v>
       </c>
-      <c r="N166" s="8">
+      <c r="N166" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8085,7 +8079,7 @@
       <c r="M167" s="3">
         <v>183.15</v>
       </c>
-      <c r="N167" s="8">
+      <c r="N167" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8130,7 +8124,7 @@
       <c r="M168" s="3">
         <v>254.8</v>
       </c>
-      <c r="N168" s="8">
+      <c r="N168" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8175,7 +8169,7 @@
       <c r="M169" s="3">
         <v>326.97000000000003</v>
       </c>
-      <c r="N169" s="8">
+      <c r="N169" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8220,7 +8214,7 @@
       <c r="M170" s="3">
         <v>403.11</v>
       </c>
-      <c r="N170" s="8">
+      <c r="N170" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8265,7 +8259,7 @@
       <c r="M171" s="3">
         <v>468.52</v>
       </c>
-      <c r="N171" s="8">
+      <c r="N171" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8310,7 +8304,7 @@
       <c r="M172" s="3">
         <v>537.79999999999995</v>
       </c>
-      <c r="N172" s="8">
+      <c r="N172" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8355,7 +8349,7 @@
       <c r="M173" s="3">
         <v>603.20000000000005</v>
       </c>
-      <c r="N173" s="8">
+      <c r="N173" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8400,7 +8394,7 @@
       <c r="M174" s="3">
         <v>681.31</v>
       </c>
-      <c r="N174" s="8">
+      <c r="N174" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8445,7 +8439,7 @@
       <c r="M175" s="3">
         <v>763.78</v>
       </c>
-      <c r="N175" s="8">
+      <c r="N175" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8490,7 +8484,7 @@
       <c r="M176" s="3">
         <v>826.11</v>
       </c>
-      <c r="N176" s="8">
+      <c r="N176" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8535,7 +8529,7 @@
       <c r="M177" s="3">
         <v>74.16</v>
       </c>
-      <c r="N177" s="8">
+      <c r="N177" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8580,7 +8574,7 @@
       <c r="M178" s="3">
         <v>152.63999999999999</v>
       </c>
-      <c r="N178" s="8">
+      <c r="N178" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8625,7 +8619,7 @@
       <c r="M179" s="3">
         <v>229.92</v>
       </c>
-      <c r="N179" s="8">
+      <c r="N179" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8670,7 +8664,7 @@
       <c r="M180" s="3">
         <v>301.97000000000003</v>
       </c>
-      <c r="N180" s="8">
+      <c r="N180" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8715,7 +8709,7 @@
       <c r="M181" s="3">
         <v>354.95</v>
       </c>
-      <c r="N181" s="8">
+      <c r="N181" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8760,7 +8754,7 @@
       <c r="M182" s="3">
         <v>402.3</v>
       </c>
-      <c r="N182" s="8">
+      <c r="N182" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8805,7 +8799,7 @@
       <c r="M183" s="3">
         <v>464.4</v>
       </c>
-      <c r="N183" s="8">
+      <c r="N183" s="5">
         <f t="shared" si="2"/>
         <v>-750.00000000000023</v>
       </c>
@@ -8850,7 +8844,7 @@
       <c r="M184" s="3">
         <v>543.72</v>
       </c>
-      <c r="N184" s="8">
+      <c r="N184" s="5">
         <f t="shared" si="2"/>
         <v>-929.99999999999977</v>
       </c>
@@ -8895,7 +8889,7 @@
       <c r="M185" s="3">
         <v>625.41</v>
       </c>
-      <c r="N185" s="8">
+      <c r="N185" s="5">
         <f t="shared" si="2"/>
         <v>-1105</v>
       </c>
@@ -8940,7 +8934,7 @@
       <c r="M186" s="3">
         <v>708.38</v>
       </c>
-      <c r="N186" s="8">
+      <c r="N186" s="5">
         <f t="shared" si="2"/>
         <v>-1226</v>
       </c>
@@ -8985,7 +8979,7 @@
       <c r="M187" s="3">
         <v>783.52</v>
       </c>
-      <c r="N187" s="8">
+      <c r="N187" s="5">
         <f t="shared" si="2"/>
         <v>-1346</v>
       </c>
@@ -9030,7 +9024,7 @@
       <c r="M188" s="3">
         <v>855.3</v>
       </c>
-      <c r="N188" s="8">
+      <c r="N188" s="5">
         <f t="shared" si="2"/>
         <v>-1442</v>
       </c>
@@ -9075,7 +9069,7 @@
       <c r="M189" s="3">
         <v>79.56</v>
       </c>
-      <c r="N189" s="8">
+      <c r="N189" s="5">
         <f t="shared" si="2"/>
         <v>-203</v>
       </c>
@@ -9120,7 +9114,7 @@
       <c r="M190" s="3">
         <v>160.25</v>
       </c>
-      <c r="N190" s="8">
+      <c r="N190" s="5">
         <f t="shared" si="2"/>
         <v>-399</v>
       </c>
@@ -9165,7 +9159,7 @@
       <c r="M191" s="3">
         <v>236.9</v>
       </c>
-      <c r="N191" s="8">
+      <c r="N191" s="5">
         <f t="shared" si="2"/>
         <v>-598</v>
       </c>
@@ -9210,7 +9204,7 @@
       <c r="M192" s="3">
         <v>305.8</v>
       </c>
-      <c r="N192" s="8">
+      <c r="N192" s="5">
         <f t="shared" si="2"/>
         <v>-946</v>
       </c>
@@ -9255,7 +9249,7 @@
       <c r="M193" s="3">
         <v>382.78</v>
       </c>
-      <c r="N193" s="8">
+      <c r="N193" s="5">
         <f t="shared" si="2"/>
         <v>-1186</v>
       </c>
@@ -9300,7 +9294,7 @@
       <c r="M194" s="3">
         <v>465.21</v>
       </c>
-      <c r="N194" s="8">
+      <c r="N194" s="5">
         <f t="shared" si="2"/>
         <v>-1475.0000000000002</v>
       </c>
@@ -9345,7 +9339,7 @@
       <c r="M195" s="3">
         <v>545.9</v>
       </c>
-      <c r="N195" s="8">
+      <c r="N195" s="5">
         <f t="shared" si="2"/>
         <v>-1661</v>
       </c>
@@ -9390,7 +9384,7 @@
       <c r="M196" s="3">
         <v>624.79</v>
       </c>
-      <c r="N196" s="8">
+      <c r="N196" s="5">
         <f t="shared" si="2"/>
         <v>-1796</v>
       </c>
@@ -9435,7 +9429,7 @@
       <c r="M197" s="3">
         <v>711.4</v>
       </c>
-      <c r="N197" s="8">
+      <c r="N197" s="5">
         <f t="shared" si="2"/>
         <v>-1945</v>
       </c>
@@ -9480,7 +9474,7 @@
       <c r="M198" s="3">
         <v>802.76</v>
       </c>
-      <c r="N198" s="8">
+      <c r="N198" s="5">
         <f t="shared" si="2"/>
         <v>-2140.9999999999995</v>
       </c>
@@ -9525,7 +9519,7 @@
       <c r="M199" s="3">
         <v>883.95</v>
       </c>
-      <c r="N199" s="8">
+      <c r="N199" s="5">
         <f t="shared" si="2"/>
         <v>-2436</v>
       </c>
@@ -9570,7 +9564,7 @@
       <c r="M200" s="3">
         <v>970.75</v>
       </c>
-      <c r="N200" s="8">
+      <c r="N200" s="5">
         <f t="shared" si="2"/>
         <v>-2642</v>
       </c>
@@ -9615,7 +9609,7 @@
       <c r="M201" s="3">
         <v>80.66</v>
       </c>
-      <c r="N201" s="8">
+      <c r="N201" s="5">
         <f t="shared" ref="N201:N264" si="3">E201-D201</f>
         <v>-227</v>
       </c>
@@ -9660,7 +9654,7 @@
       <c r="M202" s="3">
         <v>160.16</v>
       </c>
-      <c r="N202" s="8">
+      <c r="N202" s="5">
         <f t="shared" si="3"/>
         <v>-379</v>
       </c>
@@ -9705,7 +9699,7 @@
       <c r="M203" s="3">
         <v>253.43</v>
       </c>
-      <c r="N203" s="8">
+      <c r="N203" s="5">
         <f t="shared" si="3"/>
         <v>-491</v>
       </c>
@@ -9750,7 +9744,7 @@
       <c r="M204" s="3">
         <v>335.7</v>
       </c>
-      <c r="N204" s="8">
+      <c r="N204" s="5">
         <f t="shared" si="3"/>
         <v>-601</v>
       </c>
@@ -9795,7 +9789,7 @@
       <c r="M205" s="3">
         <v>417</v>
       </c>
-      <c r="N205" s="8">
+      <c r="N205" s="5">
         <f t="shared" si="3"/>
         <v>-635</v>
       </c>
@@ -9840,7 +9834,7 @@
       <c r="M206" s="3">
         <v>500.06</v>
       </c>
-      <c r="N206" s="8">
+      <c r="N206" s="5">
         <f t="shared" si="3"/>
         <v>-816.00000000000011</v>
       </c>
@@ -9885,7 +9879,7 @@
       <c r="M207" s="3">
         <v>590.44000000000005</v>
       </c>
-      <c r="N207" s="8">
+      <c r="N207" s="5">
         <f t="shared" si="3"/>
         <v>-930.00000000000023</v>
       </c>
@@ -9930,7 +9924,7 @@
       <c r="M208" s="3">
         <v>688.7</v>
       </c>
-      <c r="N208" s="8">
+      <c r="N208" s="5">
         <f t="shared" si="3"/>
         <v>-1001</v>
       </c>
@@ -9975,7 +9969,7 @@
       <c r="M209" s="3">
         <v>771.3</v>
       </c>
-      <c r="N209" s="8">
+      <c r="N209" s="5">
         <f t="shared" si="3"/>
         <v>-1169</v>
       </c>
@@ -10020,7 +10014,7 @@
       <c r="M210" s="3">
         <v>846.99</v>
       </c>
-      <c r="N210" s="8">
+      <c r="N210" s="5">
         <f t="shared" si="3"/>
         <v>-1358</v>
       </c>
@@ -10065,7 +10059,7 @@
       <c r="M211" s="3">
         <v>919.97</v>
       </c>
-      <c r="N211" s="8">
+      <c r="N211" s="5">
         <f t="shared" si="3"/>
         <v>-1523</v>
       </c>
@@ -10110,7 +10104,7 @@
       <c r="M212" s="3">
         <v>988.59</v>
       </c>
-      <c r="N212" s="8">
+      <c r="N212" s="5">
         <f t="shared" si="3"/>
         <v>-1741.9999999999995</v>
       </c>
@@ -10155,7 +10149,7 @@
       <c r="M213" s="3">
         <v>101.21</v>
       </c>
-      <c r="N213" s="8">
+      <c r="N213" s="5">
         <f t="shared" si="3"/>
         <v>-167</v>
       </c>
@@ -10200,7 +10194,7 @@
       <c r="M214" s="3">
         <v>175.81</v>
       </c>
-      <c r="N214" s="8">
+      <c r="N214" s="5">
         <f t="shared" si="3"/>
         <v>-305</v>
       </c>
@@ -10245,7 +10239,7 @@
       <c r="M215" s="3">
         <v>252.03</v>
       </c>
-      <c r="N215" s="8">
+      <c r="N215" s="5">
         <f t="shared" si="3"/>
         <v>-497</v>
       </c>
@@ -10290,7 +10284,7 @@
       <c r="M216" s="3">
         <v>313.49</v>
       </c>
-      <c r="N216" s="8">
+      <c r="N216" s="5">
         <f t="shared" si="3"/>
         <v>-696</v>
       </c>
@@ -10335,7 +10329,7 @@
       <c r="M217" s="3">
         <v>404.73</v>
       </c>
-      <c r="N217" s="8">
+      <c r="N217" s="5">
         <f t="shared" si="3"/>
         <v>-886</v>
       </c>
@@ -10380,7 +10374,7 @@
       <c r="M218" s="3">
         <v>484.23</v>
       </c>
-      <c r="N218" s="8">
+      <c r="N218" s="5">
         <f t="shared" si="3"/>
         <v>-1202.9999999999998</v>
       </c>
@@ -10425,7 +10419,7 @@
       <c r="M219" s="3">
         <v>566.25</v>
       </c>
-      <c r="N219" s="8">
+      <c r="N219" s="5">
         <f t="shared" si="3"/>
         <v>-1485</v>
       </c>
@@ -10470,7 +10464,7 @@
       <c r="M220" s="3">
         <v>647.92999999999995</v>
       </c>
-      <c r="N220" s="8">
+      <c r="N220" s="5">
         <f t="shared" si="3"/>
         <v>-1755</v>
       </c>
@@ -10515,7 +10509,7 @@
       <c r="M221" s="3">
         <v>731.52</v>
       </c>
-      <c r="N221" s="8">
+      <c r="N221" s="5">
         <f t="shared" si="3"/>
         <v>-2005</v>
       </c>
@@ -10560,7 +10554,7 @@
       <c r="M222" s="3">
         <v>813.87</v>
       </c>
-      <c r="N222" s="8">
+      <c r="N222" s="5">
         <f t="shared" si="3"/>
         <v>-2187</v>
       </c>
@@ -10605,7 +10599,7 @@
       <c r="M223" s="3">
         <v>885.41</v>
       </c>
-      <c r="N223" s="8">
+      <c r="N223" s="5">
         <f t="shared" si="3"/>
         <v>-2305.0000000000005</v>
       </c>
@@ -10650,7 +10644,7 @@
       <c r="M224" s="3">
         <v>959.95</v>
       </c>
-      <c r="N224" s="8">
+      <c r="N224" s="5">
         <f t="shared" si="3"/>
         <v>-2402.9999999999995</v>
       </c>
@@ -10695,7 +10689,7 @@
       <c r="M225" s="3">
         <v>76.48</v>
       </c>
-      <c r="N225" s="8">
+      <c r="N225" s="5">
         <f t="shared" si="3"/>
         <v>-184</v>
       </c>
@@ -10740,7 +10734,7 @@
       <c r="M226" s="3">
         <v>162.13</v>
       </c>
-      <c r="N226" s="8">
+      <c r="N226" s="5">
         <f t="shared" si="3"/>
         <v>-271</v>
       </c>
@@ -10785,7 +10779,7 @@
       <c r="M227" s="3">
         <v>253.72</v>
       </c>
-      <c r="N227" s="8">
+      <c r="N227" s="5">
         <f t="shared" si="3"/>
         <v>-415</v>
       </c>
@@ -10830,7 +10824,7 @@
       <c r="M228" s="3">
         <v>346.69</v>
       </c>
-      <c r="N228" s="8">
+      <c r="N228" s="5">
         <f t="shared" si="3"/>
         <v>-637</v>
       </c>
@@ -10875,7 +10869,7 @@
       <c r="M229" s="3">
         <v>451.97</v>
       </c>
-      <c r="N229" s="8">
+      <c r="N229" s="5">
         <f t="shared" si="3"/>
         <v>-832</v>
       </c>
@@ -10920,7 +10914,7 @@
       <c r="M230" s="3">
         <v>552.1</v>
       </c>
-      <c r="N230" s="8">
+      <c r="N230" s="5">
         <f t="shared" si="3"/>
         <v>-1014.0000000000001</v>
       </c>
@@ -10965,7 +10959,7 @@
       <c r="M231" s="3">
         <v>660.58</v>
       </c>
-      <c r="N231" s="8">
+      <c r="N231" s="5">
         <f t="shared" si="3"/>
         <v>-1276</v>
       </c>
@@ -11010,7 +11004,7 @@
       <c r="M232" s="3">
         <v>768.36</v>
       </c>
-      <c r="N232" s="8">
+      <c r="N232" s="5">
         <f t="shared" si="3"/>
         <v>-1400</v>
       </c>
@@ -11055,7 +11049,7 @@
       <c r="M233" s="3">
         <v>866.96</v>
       </c>
-      <c r="N233" s="8">
+      <c r="N233" s="5">
         <f t="shared" si="3"/>
         <v>-1498</v>
       </c>
@@ -11100,7 +11094,7 @@
       <c r="M234" s="3">
         <v>969.27</v>
       </c>
-      <c r="N234" s="8">
+      <c r="N234" s="5">
         <f t="shared" si="3"/>
         <v>-1603</v>
       </c>
@@ -11145,7 +11139,7 @@
       <c r="M235" s="3">
         <v>1061.73</v>
       </c>
-      <c r="N235" s="8">
+      <c r="N235" s="5">
         <f t="shared" si="3"/>
         <v>-1685</v>
       </c>
@@ -11190,7 +11184,7 @@
       <c r="M236" s="3">
         <v>1153.27</v>
       </c>
-      <c r="N236" s="8">
+      <c r="N236" s="5">
         <f t="shared" si="3"/>
         <v>-1829</v>
       </c>
@@ -11235,7 +11229,7 @@
       <c r="M237" s="3">
         <v>95.93</v>
       </c>
-      <c r="N237" s="8">
+      <c r="N237" s="5">
         <f t="shared" si="3"/>
         <v>-202</v>
       </c>
@@ -11280,7 +11274,7 @@
       <c r="M238" s="3">
         <v>193.24</v>
       </c>
-      <c r="N238" s="8">
+      <c r="N238" s="5">
         <f t="shared" si="3"/>
         <v>-352</v>
       </c>
@@ -11325,7 +11319,7 @@
       <c r="M239" s="3">
         <v>302.73</v>
       </c>
-      <c r="N239" s="8">
+      <c r="N239" s="5">
         <f t="shared" si="3"/>
         <v>-547</v>
       </c>
@@ -11370,7 +11364,7 @@
       <c r="M240" s="3">
         <v>402</v>
       </c>
-      <c r="N240" s="8">
+      <c r="N240" s="5">
         <f t="shared" si="3"/>
         <v>-784</v>
       </c>
@@ -11415,7 +11409,7 @@
       <c r="M241" s="3">
         <v>493.06</v>
       </c>
-      <c r="N241" s="8">
+      <c r="N241" s="5">
         <f t="shared" si="3"/>
         <v>-1086</v>
       </c>
@@ -11460,7 +11454,7 @@
       <c r="M242" s="3">
         <v>585.66999999999996</v>
       </c>
-      <c r="N242" s="8">
+      <c r="N242" s="5">
         <f t="shared" si="3"/>
         <v>-1313</v>
       </c>
@@ -11505,7 +11499,7 @@
       <c r="M243" s="3">
         <v>674.02</v>
       </c>
-      <c r="N243" s="8">
+      <c r="N243" s="5">
         <f t="shared" si="3"/>
         <v>-1586</v>
       </c>
@@ -11550,7 +11544,7 @@
       <c r="M244" s="3">
         <v>766.73</v>
       </c>
-      <c r="N244" s="8">
+      <c r="N244" s="5">
         <f t="shared" si="3"/>
         <v>-1779</v>
       </c>
@@ -11595,7 +11589,7 @@
       <c r="M245" s="3">
         <v>868.98</v>
       </c>
-      <c r="N245" s="8">
+      <c r="N245" s="5">
         <f t="shared" si="3"/>
         <v>-1898</v>
       </c>
@@ -11640,7 +11634,7 @@
       <c r="M246" s="3">
         <v>977.61</v>
       </c>
-      <c r="N246" s="8">
+      <c r="N246" s="5">
         <f t="shared" si="3"/>
         <v>-1952</v>
       </c>
@@ -11685,7 +11679,7 @@
       <c r="M247" s="3">
         <v>1074.3</v>
       </c>
-      <c r="N247" s="8">
+      <c r="N247" s="5">
         <f t="shared" si="3"/>
         <v>-2020.0000000000005</v>
       </c>
@@ -11730,7 +11724,7 @@
       <c r="M248" s="3">
         <v>1165.3699999999999</v>
       </c>
-      <c r="N248" s="8">
+      <c r="N248" s="5">
         <f t="shared" si="3"/>
         <v>-2181.9999999999995</v>
       </c>
@@ -11775,7 +11769,7 @@
       <c r="M249" s="3">
         <v>89.95</v>
       </c>
-      <c r="N249" s="8">
+      <c r="N249" s="5">
         <f t="shared" si="3"/>
         <v>-126.00000000000001</v>
       </c>
@@ -11820,7 +11814,7 @@
       <c r="M250" s="3">
         <v>187.62</v>
       </c>
-      <c r="N250" s="8">
+      <c r="N250" s="5">
         <f t="shared" si="3"/>
         <v>-314</v>
       </c>
@@ -11865,7 +11859,7 @@
       <c r="M251" s="3">
         <v>301.62</v>
       </c>
-      <c r="N251" s="8">
+      <c r="N251" s="5">
         <f t="shared" si="3"/>
         <v>-479</v>
       </c>
@@ -11910,7 +11904,7 @@
       <c r="M252" s="3">
         <v>409.46</v>
       </c>
-      <c r="N252" s="8">
+      <c r="N252" s="5">
         <f t="shared" si="3"/>
         <v>-641</v>
       </c>
@@ -11955,7 +11949,7 @@
       <c r="M253" s="3">
         <v>527.75</v>
       </c>
-      <c r="N253" s="8">
+      <c r="N253" s="5">
         <f t="shared" si="3"/>
         <v>-804</v>
       </c>
@@ -12000,7 +11994,7 @@
       <c r="M254" s="3">
         <v>657.69</v>
       </c>
-      <c r="N254" s="8">
+      <c r="N254" s="5">
         <f t="shared" si="3"/>
         <v>-915</v>
       </c>
@@ -12045,7 +12039,7 @@
       <c r="M255" s="3">
         <v>793.08</v>
       </c>
-      <c r="N255" s="8">
+      <c r="N255" s="5">
         <f t="shared" si="3"/>
         <v>-1082</v>
       </c>
@@ -12090,7 +12084,7 @@
       <c r="M256" s="3">
         <v>933.51</v>
       </c>
-      <c r="N256" s="8">
+      <c r="N256" s="5">
         <f t="shared" si="3"/>
         <v>-1114</v>
       </c>
@@ -12135,7 +12129,7 @@
       <c r="M257" s="3">
         <v>1077.07</v>
       </c>
-      <c r="N257" s="8">
+      <c r="N257" s="5">
         <f t="shared" si="3"/>
         <v>-1186</v>
       </c>
@@ -12180,7 +12174,7 @@
       <c r="M258" s="3">
         <v>1213.03</v>
       </c>
-      <c r="N258" s="8">
+      <c r="N258" s="5">
         <f t="shared" si="3"/>
         <v>-1215</v>
       </c>
@@ -12225,7 +12219,7 @@
       <c r="M259" s="3">
         <v>1343.15</v>
       </c>
-      <c r="N259" s="8">
+      <c r="N259" s="5">
         <f t="shared" si="3"/>
         <v>-1230</v>
       </c>
@@ -12270,7 +12264,7 @@
       <c r="M260" s="3">
         <v>1479.43</v>
       </c>
-      <c r="N260" s="8">
+      <c r="N260" s="5">
         <f t="shared" si="3"/>
         <v>-1192</v>
       </c>
@@ -12315,7 +12309,7 @@
       <c r="M261" s="3">
         <v>134.76859999999999</v>
       </c>
-      <c r="N261" s="8">
+      <c r="N261" s="5">
         <f t="shared" si="3"/>
         <v>15.999999999999972</v>
       </c>
@@ -12360,7 +12354,7 @@
       <c r="M262" s="3">
         <v>263.39999999999998</v>
       </c>
-      <c r="N262" s="8">
+      <c r="N262" s="5">
         <f t="shared" si="3"/>
         <v>-113</v>
       </c>
@@ -12405,7 +12399,7 @@
       <c r="M263" s="3">
         <v>402.9</v>
       </c>
-      <c r="N263" s="8">
+      <c r="N263" s="5">
         <f t="shared" si="3"/>
         <v>-171</v>
       </c>
@@ -12450,7 +12444,7 @@
       <c r="M264" s="3">
         <v>549.5</v>
       </c>
-      <c r="N264" s="8">
+      <c r="N264" s="5">
         <f t="shared" si="3"/>
         <v>-255.00000000000011</v>
       </c>
@@ -12495,7 +12489,7 @@
       <c r="M265" s="3">
         <v>695.7</v>
       </c>
-      <c r="N265" s="8">
+      <c r="N265" s="5">
         <f t="shared" ref="N265:N328" si="4">E265-D265</f>
         <v>-304</v>
       </c>
@@ -12540,7 +12534,7 @@
       <c r="M266" s="3">
         <v>842.2</v>
       </c>
-      <c r="N266" s="8">
+      <c r="N266" s="5">
         <f t="shared" si="4"/>
         <v>-420</v>
       </c>
@@ -12585,7 +12579,7 @@
       <c r="M267" s="3">
         <v>1001.2</v>
       </c>
-      <c r="N267" s="8">
+      <c r="N267" s="5">
         <f t="shared" si="4"/>
         <v>-443</v>
       </c>
@@ -12630,7 +12624,7 @@
       <c r="M268" s="3">
         <v>1151.0999999999999</v>
       </c>
-      <c r="N268" s="8">
+      <c r="N268" s="5">
         <f t="shared" si="4"/>
         <v>-492</v>
       </c>
@@ -12675,7 +12669,7 @@
       <c r="M269" s="3">
         <v>1300.7</v>
       </c>
-      <c r="N269" s="8">
+      <c r="N269" s="5">
         <f t="shared" si="4"/>
         <v>-566</v>
       </c>
@@ -12720,7 +12714,7 @@
       <c r="M270" s="3">
         <v>1443.4</v>
       </c>
-      <c r="N270" s="8">
+      <c r="N270" s="5">
         <f t="shared" si="4"/>
         <v>-650</v>
       </c>
@@ -12765,7 +12759,7 @@
       <c r="M271" s="3">
         <v>1579.1</v>
       </c>
-      <c r="N271" s="8">
+      <c r="N271" s="5">
         <f t="shared" si="4"/>
         <v>-792.99999999999955</v>
       </c>
@@ -12810,7 +12804,7 @@
       <c r="M272" s="3">
         <v>1714.7</v>
       </c>
-      <c r="N272" s="8">
+      <c r="N272" s="5">
         <f t="shared" si="4"/>
         <v>-1000.0000000000005</v>
       </c>
@@ -12855,7 +12849,7 @@
       <c r="M273" s="3">
         <v>141.8937</v>
       </c>
-      <c r="N273" s="8">
+      <c r="N273" s="5">
         <f t="shared" si="4"/>
         <v>-170.99999999999997</v>
       </c>
@@ -12900,7 +12894,7 @@
       <c r="M274" s="3">
         <v>283.89999999999998</v>
       </c>
-      <c r="N274" s="8">
+      <c r="N274" s="5">
         <f t="shared" si="4"/>
         <v>-315</v>
       </c>
@@ -12945,7 +12939,7 @@
       <c r="M275" s="3">
         <v>429.6</v>
       </c>
-      <c r="N275" s="8">
+      <c r="N275" s="5">
         <f t="shared" si="4"/>
         <v>-445</v>
       </c>
@@ -12990,7 +12984,7 @@
       <c r="M276" s="3">
         <v>584.20000000000005</v>
       </c>
-      <c r="N276" s="8">
+      <c r="N276" s="5">
         <f t="shared" si="4"/>
         <v>-562</v>
       </c>
@@ -13035,7 +13029,7 @@
       <c r="M277" s="3">
         <v>749.4</v>
       </c>
-      <c r="N277" s="8">
+      <c r="N277" s="5">
         <f t="shared" si="4"/>
         <v>-654</v>
       </c>
@@ -13080,7 +13074,7 @@
       <c r="M278" s="3">
         <v>897.7</v>
       </c>
-      <c r="N278" s="8">
+      <c r="N278" s="5">
         <f t="shared" si="4"/>
         <v>-789</v>
       </c>
@@ -13125,7 +13119,7 @@
       <c r="M279" s="3">
         <v>1066.7</v>
       </c>
-      <c r="N279" s="8">
+      <c r="N279" s="5">
         <f t="shared" si="4"/>
         <v>-868.99999999999977</v>
       </c>
@@ -13170,7 +13164,7 @@
       <c r="M280" s="3">
         <v>1236</v>
       </c>
-      <c r="N280" s="8">
+      <c r="N280" s="5">
         <f t="shared" si="4"/>
         <v>-999</v>
       </c>
@@ -13215,7 +13209,7 @@
       <c r="M281" s="3">
         <v>1405.6</v>
       </c>
-      <c r="N281" s="8">
+      <c r="N281" s="5">
         <f t="shared" si="4"/>
         <v>-1055.0000000000005</v>
       </c>
@@ -13260,7 +13254,7 @@
       <c r="M282" s="3">
         <v>1552.9</v>
       </c>
-      <c r="N282" s="8">
+      <c r="N282" s="5">
         <f t="shared" si="4"/>
         <v>-1186.9999999999995</v>
       </c>
@@ -13305,7 +13299,7 @@
       <c r="M283" s="3">
         <v>1716.1</v>
       </c>
-      <c r="N283" s="8">
+      <c r="N283" s="5">
         <f t="shared" si="4"/>
         <v>-1311</v>
       </c>
@@ -13350,7 +13344,7 @@
       <c r="M284" s="3">
         <v>1879.8</v>
       </c>
-      <c r="N284" s="8">
+      <c r="N284" s="5">
         <f t="shared" si="4"/>
         <v>-1489.9999999999995</v>
       </c>
@@ -13395,7 +13389,7 @@
       <c r="M285" s="3">
         <v>176.7972</v>
       </c>
-      <c r="N285" s="8">
+      <c r="N285" s="5">
         <f t="shared" si="4"/>
         <v>-109</v>
       </c>
@@ -13440,7 +13434,7 @@
       <c r="M286" s="3">
         <v>344.4</v>
       </c>
-      <c r="N286" s="8">
+      <c r="N286" s="5">
         <f t="shared" si="4"/>
         <v>-288</v>
       </c>
@@ -13485,7 +13479,7 @@
       <c r="M287" s="3">
         <v>509.5</v>
       </c>
-      <c r="N287" s="8">
+      <c r="N287" s="5">
         <f t="shared" si="4"/>
         <v>-474</v>
       </c>
@@ -13530,7 +13524,7 @@
       <c r="M288" s="3">
         <v>677.2</v>
       </c>
-      <c r="N288" s="8">
+      <c r="N288" s="5">
         <f t="shared" si="4"/>
         <v>-609</v>
       </c>
@@ -13575,7 +13569,7 @@
       <c r="M289" s="3">
         <v>853.7</v>
       </c>
-      <c r="N289" s="8">
+      <c r="N289" s="5">
         <f t="shared" si="4"/>
         <v>-749.00000000000023</v>
       </c>
@@ -13620,7 +13614,7 @@
       <c r="M290" s="3">
         <v>1017.4</v>
       </c>
-      <c r="N290" s="8">
+      <c r="N290" s="5">
         <f t="shared" si="4"/>
         <v>-836</v>
       </c>
@@ -13665,7 +13659,7 @@
       <c r="M291" s="3">
         <v>1188.4000000000001</v>
       </c>
-      <c r="N291" s="8">
+      <c r="N291" s="5">
         <f t="shared" si="4"/>
         <v>-968</v>
       </c>
@@ -13710,7 +13704,7 @@
       <c r="M292" s="3">
         <v>1373.2</v>
       </c>
-      <c r="N292" s="8">
+      <c r="N292" s="5">
         <f t="shared" si="4"/>
         <v>-981.99999999999977</v>
       </c>
@@ -13755,7 +13749,7 @@
       <c r="M293" s="3">
         <v>1566.2</v>
       </c>
-      <c r="N293" s="8">
+      <c r="N293" s="5">
         <f t="shared" si="4"/>
         <v>-1116.9999999999998</v>
       </c>
@@ -13800,7 +13794,7 @@
       <c r="M294" s="3">
         <v>1752.7</v>
       </c>
-      <c r="N294" s="8">
+      <c r="N294" s="5">
         <f t="shared" si="4"/>
         <v>-1255</v>
       </c>
@@ -13845,7 +13839,7 @@
       <c r="M295" s="3">
         <v>1941.3</v>
       </c>
-      <c r="N295" s="8">
+      <c r="N295" s="5">
         <f t="shared" si="4"/>
         <v>-1389</v>
       </c>
@@ -13890,7 +13884,7 @@
       <c r="M296" s="3">
         <v>2131.4</v>
       </c>
-      <c r="N296" s="8">
+      <c r="N296" s="5">
         <f t="shared" si="4"/>
         <v>-1553</v>
       </c>
@@ -13935,7 +13929,7 @@
       <c r="M297" s="3">
         <v>197.3</v>
       </c>
-      <c r="N297" s="8">
+      <c r="N297" s="5">
         <f t="shared" si="4"/>
         <v>-148</v>
       </c>
@@ -13980,7 +13974,7 @@
       <c r="M298" s="3">
         <v>384.1</v>
       </c>
-      <c r="N298" s="8">
+      <c r="N298" s="5">
         <f t="shared" si="4"/>
         <v>-267</v>
       </c>
@@ -14025,7 +14019,7 @@
       <c r="M299" s="3">
         <v>582.1</v>
       </c>
-      <c r="N299" s="8">
+      <c r="N299" s="5">
         <f t="shared" si="4"/>
         <v>-315</v>
       </c>
@@ -14070,7 +14064,7 @@
       <c r="M300" s="3">
         <v>777.3</v>
       </c>
-      <c r="N300" s="8">
+      <c r="N300" s="5">
         <f t="shared" si="4"/>
         <v>-436</v>
       </c>
@@ -14115,7 +14109,7 @@
       <c r="M301" s="3">
         <v>991.1</v>
       </c>
-      <c r="N301" s="8">
+      <c r="N301" s="5">
         <f t="shared" si="4"/>
         <v>-562</v>
       </c>
@@ -14160,7 +14154,7 @@
       <c r="M302" s="3">
         <v>1190.83</v>
       </c>
-      <c r="N302" s="8">
+      <c r="N302" s="5">
         <f t="shared" si="4"/>
         <v>-690</v>
       </c>
@@ -14205,7 +14199,7 @@
       <c r="M303" s="3">
         <v>1395.05</v>
       </c>
-      <c r="N303" s="8">
+      <c r="N303" s="5">
         <f t="shared" si="4"/>
         <v>-812</v>
       </c>
@@ -14250,7 +14244,7 @@
       <c r="M304" s="3">
         <v>1621.39</v>
       </c>
-      <c r="N304" s="8">
+      <c r="N304" s="5">
         <f t="shared" si="4"/>
         <v>-820</v>
       </c>
@@ -14295,7 +14289,7 @@
       <c r="M305" s="3">
         <v>1845.69</v>
       </c>
-      <c r="N305" s="8">
+      <c r="N305" s="5">
         <f t="shared" si="4"/>
         <v>-910</v>
       </c>
@@ -14340,7 +14334,7 @@
       <c r="M306" s="3">
         <v>2078.4499999999998</v>
       </c>
-      <c r="N306" s="8">
+      <c r="N306" s="5">
         <f t="shared" si="4"/>
         <v>-962.00000000000045</v>
       </c>
@@ -14385,7 +14379,7 @@
       <c r="M307" s="3">
         <v>2284.65</v>
       </c>
-      <c r="N307" s="8">
+      <c r="N307" s="5">
         <f t="shared" si="4"/>
         <v>-1034</v>
       </c>
@@ -14430,7 +14424,7 @@
       <c r="M308" s="3">
         <v>2509.64</v>
       </c>
-      <c r="N308" s="8">
+      <c r="N308" s="5">
         <f t="shared" si="4"/>
         <v>-1108</v>
       </c>
@@ -14475,7 +14469,7 @@
       <c r="M309" s="3">
         <v>229.19</v>
       </c>
-      <c r="N309" s="8">
+      <c r="N309" s="5">
         <f t="shared" si="4"/>
         <v>-150.66409999999999</v>
       </c>
@@ -14520,7 +14514,7 @@
       <c r="M310" s="3">
         <v>459.6</v>
       </c>
-      <c r="N310" s="8">
+      <c r="N310" s="5">
         <f t="shared" si="4"/>
         <v>-190.41880000000003</v>
       </c>
@@ -14565,7 +14559,7 @@
       <c r="M311" s="3">
         <v>703.4</v>
       </c>
-      <c r="N311" s="8">
+      <c r="N311" s="5">
         <f t="shared" si="4"/>
         <v>-153.30359999999996</v>
       </c>
@@ -14610,7 +14604,7 @@
       <c r="M312" s="3">
         <v>945</v>
       </c>
-      <c r="N312" s="8">
+      <c r="N312" s="5">
         <f t="shared" si="4"/>
         <v>-188.1925</v>
       </c>
@@ -14655,7 +14649,7 @@
       <c r="M313" s="3">
         <v>1190</v>
       </c>
-      <c r="N313" s="8">
+      <c r="N313" s="5">
         <f t="shared" si="4"/>
         <v>-147.42229999999995</v>
       </c>
@@ -14700,7 +14694,7 @@
       <c r="M314" s="3">
         <v>1441.67</v>
       </c>
-      <c r="N314" s="8">
+      <c r="N314" s="5">
         <f t="shared" si="4"/>
         <v>-159.2675999999999</v>
       </c>
@@ -14745,7 +14739,7 @@
       <c r="M315" s="3">
         <v>1698.53</v>
       </c>
-      <c r="N315" s="8">
+      <c r="N315" s="5">
         <f t="shared" si="4"/>
         <v>-73.924400000000105</v>
       </c>
@@ -14790,7 +14784,7 @@
       <c r="M316" s="3">
         <v>1972.83</v>
       </c>
-      <c r="N316" s="8">
+      <c r="N316" s="5">
         <f t="shared" si="4"/>
         <v>-53.65339999999992</v>
       </c>
@@ -14835,7 +14829,7 @@
       <c r="M317" s="3">
         <v>2236</v>
       </c>
-      <c r="N317" s="8">
+      <c r="N317" s="5">
         <f t="shared" si="4"/>
         <v>-85.489300000000185</v>
       </c>
@@ -14880,7 +14874,7 @@
       <c r="M318" s="3">
         <v>2481.8000000000002</v>
       </c>
-      <c r="N318" s="8">
+      <c r="N318" s="5">
         <f t="shared" si="4"/>
         <v>0.78120000000035361</v>
       </c>
@@ -14925,7 +14919,7 @@
       <c r="M319" s="3">
         <v>2727.9</v>
       </c>
-      <c r="N319" s="8">
+      <c r="N319" s="5">
         <f t="shared" si="4"/>
         <v>7.6293000000000575</v>
       </c>
@@ -14970,7 +14964,7 @@
       <c r="M320" s="3">
         <v>3001</v>
       </c>
-      <c r="N320" s="8">
+      <c r="N320" s="5">
         <f t="shared" si="4"/>
         <v>-32.30560000000014</v>
       </c>
@@ -15015,7 +15009,7 @@
       <c r="M321" s="3">
         <v>279.33</v>
       </c>
-      <c r="N321" s="8">
+      <c r="N321" s="5">
         <f t="shared" si="4"/>
         <v>-27.227899999999977</v>
       </c>
@@ -15060,7 +15054,7 @@
       <c r="M322" s="3">
         <v>555.30999999999995</v>
       </c>
-      <c r="N322" s="8">
+      <c r="N322" s="5">
         <f t="shared" si="4"/>
         <v>-127.42419999999998</v>
       </c>
@@ -15105,7 +15099,7 @@
       <c r="M323" s="3">
         <v>866.8</v>
       </c>
-      <c r="N323" s="8">
+      <c r="N323" s="5">
         <f t="shared" si="4"/>
         <v>-131.78150000000005</v>
       </c>
@@ -15150,7 +15144,7 @@
       <c r="M324" s="3">
         <v>1157.3</v>
       </c>
-      <c r="N324" s="8">
+      <c r="N324" s="5">
         <f t="shared" si="4"/>
         <v>-107.58240000000023</v>
       </c>
@@ -15195,7 +15189,7 @@
       <c r="M325" s="3">
         <v>1458</v>
       </c>
-      <c r="N325" s="8">
+      <c r="N325" s="5">
         <f t="shared" si="4"/>
         <v>-95.890899999999874</v>
       </c>
@@ -15240,7 +15234,7 @@
       <c r="M326" s="3">
         <v>1758.9</v>
       </c>
-      <c r="N326" s="8">
+      <c r="N326" s="5">
         <f t="shared" si="4"/>
         <v>-100.39650000000006</v>
       </c>
@@ -15285,7 +15279,7 @@
       <c r="M327" s="3">
         <v>2071.9</v>
       </c>
-      <c r="N327" s="8">
+      <c r="N327" s="5">
         <f t="shared" si="4"/>
         <v>-38.647600000000239</v>
       </c>
@@ -15330,7 +15324,7 @@
       <c r="M328" s="3">
         <v>2384.4</v>
       </c>
-      <c r="N328" s="8">
+      <c r="N328" s="5">
         <f t="shared" si="4"/>
         <v>41.420700000000124</v>
       </c>
@@ -15375,7 +15369,7 @@
       <c r="M329" s="3">
         <v>2692.4</v>
       </c>
-      <c r="N329" s="8">
+      <c r="N329" s="5">
         <f t="shared" ref="N329:N392" si="5">E329-D329</f>
         <v>125.94610000000011</v>
       </c>
@@ -15420,7 +15414,7 @@
       <c r="M330" s="3">
         <v>3010.2764999999999</v>
       </c>
-      <c r="N330" s="8">
+      <c r="N330" s="5">
         <f t="shared" si="5"/>
         <v>254.89940000000024</v>
       </c>
@@ -15465,7 +15459,7 @@
       <c r="M331" s="3">
         <v>3323.6</v>
       </c>
-      <c r="N331" s="8">
+      <c r="N331" s="5">
         <f t="shared" si="5"/>
         <v>477.39849999999979</v>
       </c>
@@ -15510,7 +15504,7 @@
       <c r="M332" s="3">
         <v>3658.6244000000002</v>
       </c>
-      <c r="N332" s="8">
+      <c r="N332" s="5">
         <f t="shared" si="5"/>
         <v>625.69810000000007</v>
       </c>
@@ -15555,7 +15549,7 @@
       <c r="M333" s="3">
         <v>0</v>
       </c>
-      <c r="N333" s="8">
+      <c r="N333" s="5">
         <f t="shared" si="5"/>
         <v>35</v>
       </c>
@@ -15600,7 +15594,7 @@
       <c r="M334" s="3">
         <v>614.79999999999995</v>
       </c>
-      <c r="N334" s="8">
+      <c r="N334" s="5">
         <f t="shared" si="5"/>
         <v>70</v>
       </c>
@@ -15645,7 +15639,7 @@
       <c r="M335" s="3">
         <v>947.48270000000002</v>
       </c>
-      <c r="N335" s="8">
+      <c r="N335" s="5">
         <f t="shared" si="5"/>
         <v>200.00000000000011</v>
       </c>
@@ -15690,7 +15684,7 @@
       <c r="M336" s="3">
         <v>1265.4000000000001</v>
       </c>
-      <c r="N336" s="8">
+      <c r="N336" s="5">
         <f t="shared" si="5"/>
         <v>319</v>
       </c>
@@ -15735,7 +15729,7 @@
       <c r="M337" s="3">
         <v>1596.3</v>
       </c>
-      <c r="N337" s="8">
+      <c r="N337" s="5">
         <f t="shared" si="5"/>
         <v>398</v>
       </c>
@@ -15780,7 +15774,7 @@
       <c r="M338" s="3">
         <v>1928.7</v>
       </c>
-      <c r="N338" s="8">
+      <c r="N338" s="5">
         <f t="shared" si="5"/>
         <v>600</v>
       </c>
@@ -15825,7 +15819,7 @@
       <c r="M339" s="3">
         <v>2272.8000000000002</v>
       </c>
-      <c r="N339" s="8">
+      <c r="N339" s="5">
         <f t="shared" si="5"/>
         <v>848.00000000000023</v>
       </c>
@@ -15870,7 +15864,7 @@
       <c r="M340" s="3">
         <v>2618</v>
       </c>
-      <c r="N340" s="8">
+      <c r="N340" s="5">
         <f t="shared" si="5"/>
         <v>1018</v>
       </c>
@@ -15915,7 +15909,7 @@
       <c r="M341" s="3">
         <v>2945.9</v>
       </c>
-      <c r="N341" s="8">
+      <c r="N341" s="5">
         <f t="shared" si="5"/>
         <v>1255</v>
       </c>
@@ -15960,7 +15954,7 @@
       <c r="M342" s="3">
         <v>3298.3</v>
       </c>
-      <c r="N342" s="8">
+      <c r="N342" s="5">
         <f t="shared" si="5"/>
         <v>1485</v>
       </c>
@@ -16005,7 +15999,7 @@
       <c r="M343" s="3">
         <v>3644.8</v>
       </c>
-      <c r="N343" s="8">
+      <c r="N343" s="5">
         <f t="shared" si="5"/>
         <v>1770</v>
       </c>
@@ -16050,7 +16044,7 @@
       <c r="M344" s="3">
         <v>3983.8</v>
       </c>
-      <c r="N344" s="8">
+      <c r="N344" s="5">
         <f t="shared" si="5"/>
         <v>2047</v>
       </c>
@@ -16095,7 +16089,7 @@
       <c r="M345" s="3">
         <v>0</v>
       </c>
-      <c r="N345" s="8">
+      <c r="N345" s="5">
         <f t="shared" si="5"/>
         <v>44</v>
       </c>
@@ -16140,7 +16134,7 @@
       <c r="M346" s="3">
         <v>687.4</v>
       </c>
-      <c r="N346" s="8">
+      <c r="N346" s="5">
         <f t="shared" si="5"/>
         <v>232</v>
       </c>
@@ -16185,7 +16179,7 @@
       <c r="M347" s="3">
         <v>1036.4000000000001</v>
       </c>
-      <c r="N347" s="8">
+      <c r="N347" s="5">
         <f t="shared" si="5"/>
         <v>428</v>
       </c>
@@ -16230,7 +16224,7 @@
       <c r="M348" s="3">
         <v>1361.5</v>
       </c>
-      <c r="N348" s="8">
+      <c r="N348" s="5">
         <f t="shared" si="5"/>
         <v>526.99999999999989</v>
       </c>
@@ -16275,7 +16269,7 @@
       <c r="M349" s="3">
         <v>1699.8</v>
       </c>
-      <c r="N349" s="8">
+      <c r="N349" s="5">
         <f t="shared" si="5"/>
         <v>677.99999999999977</v>
       </c>
@@ -16320,7 +16314,7 @@
       <c r="M350" s="3">
         <v>2042</v>
       </c>
-      <c r="N350" s="8">
+      <c r="N350" s="5">
         <f t="shared" si="5"/>
         <v>863</v>
       </c>
@@ -16365,7 +16359,7 @@
       <c r="M351" s="3">
         <v>2387.9</v>
       </c>
-      <c r="N351" s="8">
+      <c r="N351" s="5">
         <f t="shared" si="5"/>
         <v>1083</v>
       </c>
@@ -16410,7 +16404,7 @@
       <c r="M352" s="3">
         <v>2751.4</v>
       </c>
-      <c r="N352" s="8">
+      <c r="N352" s="5">
         <f t="shared" si="5"/>
         <v>1270.0000000000002</v>
       </c>
@@ -16455,7 +16449,7 @@
       <c r="M353" s="3">
         <v>3140.7</v>
       </c>
-      <c r="N353" s="8">
+      <c r="N353" s="5">
         <f t="shared" si="5"/>
         <v>1421.9999999999995</v>
       </c>
@@ -16500,7 +16494,7 @@
       <c r="M354" s="3">
         <v>3524.4</v>
       </c>
-      <c r="N354" s="8">
+      <c r="N354" s="5">
         <f t="shared" si="5"/>
         <v>1600</v>
       </c>
@@ -16545,7 +16539,7 @@
       <c r="M355" s="3">
         <v>3883.7</v>
       </c>
-      <c r="N355" s="8">
+      <c r="N355" s="5">
         <f t="shared" si="5"/>
         <v>1921</v>
       </c>
@@ -16590,7 +16584,7 @@
       <c r="M356" s="3">
         <v>4230.8999999999996</v>
       </c>
-      <c r="N356" s="8">
+      <c r="N356" s="5">
         <f t="shared" si="5"/>
         <v>2252</v>
       </c>
@@ -16635,7 +16629,7 @@
       <c r="M357" s="3">
         <v>0</v>
       </c>
-      <c r="N357" s="8">
+      <c r="N357" s="5">
         <f t="shared" si="5"/>
         <v>125.00000000000006</v>
       </c>
@@ -16680,7 +16674,7 @@
       <c r="M358" s="3">
         <v>706.5</v>
       </c>
-      <c r="N358" s="8">
+      <c r="N358" s="5">
         <f t="shared" si="5"/>
         <v>212.00000000000011</v>
       </c>
@@ -16725,7 +16719,7 @@
       <c r="M359" s="3">
         <v>1149.5</v>
       </c>
-      <c r="N359" s="8">
+      <c r="N359" s="5">
         <f t="shared" si="5"/>
         <v>605.99999999999989</v>
       </c>
@@ -16770,7 +16764,7 @@
       <c r="M360" s="3">
         <v>1535.7</v>
       </c>
-      <c r="N360" s="8">
+      <c r="N360" s="5">
         <f t="shared" si="5"/>
         <v>817</v>
       </c>
@@ -16815,7 +16809,7 @@
       <c r="M361" s="3">
         <v>1943.2</v>
       </c>
-      <c r="N361" s="8">
+      <c r="N361" s="5">
         <f t="shared" si="5"/>
         <v>1128</v>
       </c>
@@ -16860,7 +16854,7 @@
       <c r="M362" s="3">
         <v>2347.3000000000002</v>
       </c>
-      <c r="N362" s="8">
+      <c r="N362" s="5">
         <f t="shared" si="5"/>
         <v>1384</v>
       </c>
@@ -16905,7 +16899,7 @@
       <c r="M363" s="3">
         <v>2761.1</v>
       </c>
-      <c r="N363" s="8">
+      <c r="N363" s="5">
         <f t="shared" si="5"/>
         <v>1575.0000000000002</v>
       </c>
@@ -16950,7 +16944,7 @@
       <c r="M364" s="3">
         <v>3172.4</v>
       </c>
-      <c r="N364" s="8">
+      <c r="N364" s="5">
         <f t="shared" si="5"/>
         <v>1836.9999999999995</v>
       </c>
@@ -16995,7 +16989,7 @@
       <c r="M365" s="3">
         <v>3591.4</v>
       </c>
-      <c r="N365" s="8">
+      <c r="N365" s="5">
         <f t="shared" si="5"/>
         <v>1951</v>
       </c>
@@ -17040,7 +17034,7 @@
       <c r="M366" s="3">
         <v>3985.5</v>
       </c>
-      <c r="N366" s="8">
+      <c r="N366" s="5">
         <f t="shared" si="5"/>
         <v>2095</v>
       </c>
@@ -17085,7 +17079,7 @@
       <c r="M367" s="3">
         <v>4370</v>
       </c>
-      <c r="N367" s="8">
+      <c r="N367" s="5">
         <f t="shared" si="5"/>
         <v>2232</v>
       </c>
@@ -17130,7 +17124,7 @@
       <c r="M368" s="3">
         <v>4770.3</v>
       </c>
-      <c r="N368" s="8">
+      <c r="N368" s="5">
         <f t="shared" si="5"/>
         <v>2516</v>
       </c>
@@ -17175,7 +17169,7 @@
       <c r="M369" s="3">
         <v>0</v>
       </c>
-      <c r="N369" s="8">
+      <c r="N369" s="5">
         <f t="shared" si="5"/>
         <v>204</v>
       </c>
@@ -17220,7 +17214,7 @@
       <c r="M370" s="3">
         <v>796</v>
       </c>
-      <c r="N370" s="8">
+      <c r="N370" s="5">
         <f t="shared" si="5"/>
         <v>351</v>
       </c>
@@ -17265,7 +17259,7 @@
       <c r="M371" s="3">
         <v>1218.5999999999999</v>
       </c>
-      <c r="N371" s="8">
+      <c r="N371" s="5">
         <f t="shared" si="5"/>
         <v>771.00000000000011</v>
       </c>
@@ -17310,7 +17304,7 @@
       <c r="M372" s="3">
         <v>1637.7</v>
       </c>
-      <c r="N372" s="8">
+      <c r="N372" s="5">
         <f t="shared" si="5"/>
         <v>1039</v>
       </c>
@@ -17355,7 +17349,7 @@
       <c r="M373" s="3">
         <v>2065.3000000000002</v>
       </c>
-      <c r="N373" s="8">
+      <c r="N373" s="5">
         <f t="shared" si="5"/>
         <v>1230</v>
       </c>
@@ -17400,7 +17394,7 @@
       <c r="M374" s="3">
         <v>2509.8000000000002</v>
       </c>
-      <c r="N374" s="8">
+      <c r="N374" s="5">
         <f t="shared" si="5"/>
         <v>1574.0000000000002</v>
       </c>
@@ -17445,7 +17439,7 @@
       <c r="M375" s="3">
         <v>2954.8</v>
       </c>
-      <c r="N375" s="8">
+      <c r="N375" s="5">
         <f t="shared" si="5"/>
         <v>1959.9999999999993</v>
       </c>
@@ -17490,7 +17484,7 @@
       <c r="M376" s="3">
         <v>3429.5</v>
       </c>
-      <c r="N376" s="8">
+      <c r="N376" s="5">
         <f t="shared" si="5"/>
         <v>2159</v>
       </c>
@@ -17535,7 +17529,7 @@
       <c r="M377" s="3">
         <v>3903</v>
       </c>
-      <c r="N377" s="8">
+      <c r="N377" s="5">
         <f t="shared" si="5"/>
         <v>2512</v>
       </c>
@@ -17580,7 +17574,7 @@
       <c r="M378" s="3">
         <v>4375.1000000000004</v>
       </c>
-      <c r="N378" s="8">
+      <c r="N378" s="5">
         <f t="shared" si="5"/>
         <v>2790</v>
       </c>
@@ -17625,7 +17619,7 @@
       <c r="M379" s="3">
         <v>4825</v>
       </c>
-      <c r="N379" s="8">
+      <c r="N379" s="5">
         <f t="shared" si="5"/>
         <v>3281</v>
       </c>
@@ -17670,7 +17664,7 @@
       <c r="M380" s="3">
         <v>5272.6</v>
       </c>
-      <c r="N380" s="8">
+      <c r="N380" s="5">
         <f t="shared" si="5"/>
         <v>3629</v>
       </c>
@@ -17715,7 +17709,7 @@
       <c r="M381" s="3">
         <v>0</v>
       </c>
-      <c r="N381" s="8">
+      <c r="N381" s="5">
         <f t="shared" si="5"/>
         <v>298</v>
       </c>
@@ -17760,7 +17754,7 @@
       <c r="M382" s="3">
         <v>761</v>
       </c>
-      <c r="N382" s="8">
+      <c r="N382" s="5">
         <f t="shared" si="5"/>
         <v>581</v>
       </c>
@@ -17805,7 +17799,7 @@
       <c r="M383" s="3">
         <v>1048.9000000000001</v>
       </c>
-      <c r="N383" s="8">
+      <c r="N383" s="5">
         <f t="shared" si="5"/>
         <v>1091</v>
       </c>
@@ -17850,7 +17844,7 @@
       <c r="M384" s="3">
         <v>1291.3</v>
       </c>
-      <c r="N384" s="8">
+      <c r="N384" s="5">
         <f t="shared" si="5"/>
         <v>1640</v>
       </c>
@@ -17895,7 +17889,7 @@
       <c r="M385" s="3">
         <v>1580.7</v>
       </c>
-      <c r="N385" s="8">
+      <c r="N385" s="5">
         <f t="shared" si="5"/>
         <v>1650</v>
       </c>
@@ -17940,7 +17934,7 @@
       <c r="M386" s="3">
         <v>1895.8</v>
       </c>
-      <c r="N386" s="8">
+      <c r="N386" s="5">
         <f t="shared" si="5"/>
         <v>1686</v>
       </c>
@@ -17985,7 +17979,7 @@
       <c r="M387" s="3">
         <v>2227.9</v>
       </c>
-      <c r="N387" s="8">
+      <c r="N387" s="5">
         <f t="shared" si="5"/>
         <v>1815.0000000000005</v>
       </c>
@@ -18030,7 +18024,7 @@
       <c r="M388" s="3">
         <v>2570.1</v>
       </c>
-      <c r="N388" s="8">
+      <c r="N388" s="5">
         <f t="shared" si="5"/>
         <v>2048</v>
       </c>
@@ -18075,7 +18069,7 @@
       <c r="M389" s="3">
         <v>2931.7</v>
       </c>
-      <c r="N389" s="8">
+      <c r="N389" s="5">
         <f t="shared" si="5"/>
         <v>2256</v>
       </c>
@@ -18120,7 +18114,7 @@
       <c r="M390" s="3">
         <v>3306.3</v>
       </c>
-      <c r="N390" s="8">
+      <c r="N390" s="5">
         <f t="shared" si="5"/>
         <v>2685</v>
       </c>
@@ -18165,7 +18159,7 @@
       <c r="M391" s="3">
         <v>3674.2</v>
       </c>
-      <c r="N391" s="8">
+      <c r="N391" s="5">
         <f t="shared" si="5"/>
         <v>2975</v>
       </c>
@@ -18210,7 +18204,7 @@
       <c r="M392" s="3">
         <v>4049.4</v>
       </c>
-      <c r="N392" s="8">
+      <c r="N392" s="5">
         <f t="shared" si="5"/>
         <v>3348</v>
       </c>
@@ -18255,7 +18249,7 @@
       <c r="M393" s="3">
         <v>0</v>
       </c>
-      <c r="N393" s="8">
+      <c r="N393" s="5">
         <f t="shared" ref="N393:N425" si="6">E393-D393</f>
         <v>378</v>
       </c>
@@ -18300,7 +18294,7 @@
       <c r="M394" s="3">
         <v>681.8</v>
       </c>
-      <c r="N394" s="8">
+      <c r="N394" s="5">
         <f t="shared" si="6"/>
         <v>698</v>
       </c>
@@ -18345,7 +18339,7 @@
       <c r="M395" s="3">
         <v>1045.7</v>
       </c>
-      <c r="N395" s="8">
+      <c r="N395" s="5">
         <f t="shared" si="6"/>
         <v>1171</v>
       </c>
@@ -18390,7 +18384,7 @@
       <c r="M396" s="3">
         <v>1439.6</v>
       </c>
-      <c r="N396" s="8">
+      <c r="N396" s="5">
         <f t="shared" si="6"/>
         <v>1657</v>
       </c>
@@ -18435,7 +18429,7 @@
       <c r="M397" s="3">
         <v>1871.5</v>
       </c>
-      <c r="N397" s="8">
+      <c r="N397" s="5">
         <f t="shared" si="6"/>
         <v>1964</v>
       </c>
@@ -18480,7 +18474,7 @@
       <c r="M398" s="3">
         <v>2283.4</v>
       </c>
-      <c r="N398" s="8">
+      <c r="N398" s="5">
         <f t="shared" si="6"/>
         <v>2394</v>
       </c>
@@ -18525,7 +18519,7 @@
       <c r="M399" s="3">
         <v>2632.6</v>
       </c>
-      <c r="N399" s="8">
+      <c r="N399" s="5">
         <f t="shared" si="6"/>
         <v>2604</v>
       </c>
@@ -18570,7 +18564,7 @@
       <c r="M400" s="3">
         <v>2912.6</v>
       </c>
-      <c r="N400" s="8">
+      <c r="N400" s="5">
         <f t="shared" si="6"/>
         <v>2685</v>
       </c>
@@ -18615,7 +18609,7 @@
       <c r="M401" s="3">
         <v>3219.5</v>
       </c>
-      <c r="N401" s="8">
+      <c r="N401" s="5">
         <f t="shared" si="6"/>
         <v>2876</v>
       </c>
@@ -18660,7 +18654,7 @@
       <c r="M402" s="3">
         <v>3528.2</v>
       </c>
-      <c r="N402" s="8">
+      <c r="N402" s="5">
         <f t="shared" si="6"/>
         <v>3055</v>
       </c>
@@ -18705,7 +18699,7 @@
       <c r="M403" s="3">
         <v>3754.6</v>
       </c>
-      <c r="N403" s="8">
+      <c r="N403" s="5">
         <f t="shared" si="6"/>
         <v>3216</v>
       </c>
@@ -18750,7 +18744,7 @@
       <c r="M404" s="3">
         <v>3943.9</v>
       </c>
-      <c r="N404" s="8">
+      <c r="N404" s="5">
         <f t="shared" si="6"/>
         <v>3319</v>
       </c>
@@ -18795,7 +18789,7 @@
       <c r="M405" s="3">
         <v>0</v>
       </c>
-      <c r="N405" s="8">
+      <c r="N405" s="5">
         <f t="shared" si="6"/>
         <v>148.00000000000006</v>
       </c>
@@ -18840,7 +18834,7 @@
       <c r="M406" s="3">
         <v>556.29999999999995</v>
       </c>
-      <c r="N406" s="8">
+      <c r="N406" s="5">
         <f t="shared" si="6"/>
         <v>265</v>
       </c>
@@ -18885,7 +18879,7 @@
       <c r="M407" s="3">
         <v>819</v>
       </c>
-      <c r="N407" s="8">
+      <c r="N407" s="5">
         <f t="shared" si="6"/>
         <v>486</v>
       </c>
@@ -18930,7 +18924,7 @@
       <c r="M408" s="3">
         <v>994</v>
       </c>
-      <c r="N408" s="8">
+      <c r="N408" s="5">
         <f t="shared" si="6"/>
         <v>719.99999999999977</v>
       </c>
@@ -18975,7 +18969,7 @@
       <c r="M409" s="3">
         <v>1146.2</v>
       </c>
-      <c r="N409" s="8">
+      <c r="N409" s="5">
         <f t="shared" si="6"/>
         <v>847.00000000000011</v>
       </c>
@@ -19020,7 +19014,7 @@
       <c r="M410" s="3">
         <v>1357.8</v>
       </c>
-      <c r="N410" s="8">
+      <c r="N410" s="5">
         <f t="shared" si="6"/>
         <v>1000</v>
       </c>
@@ -19065,7 +19059,7 @@
       <c r="M411" s="3">
         <v>1605.1</v>
       </c>
-      <c r="N411" s="8">
+      <c r="N411" s="5">
         <f t="shared" si="6"/>
         <v>1183</v>
       </c>
@@ -19110,7 +19104,7 @@
       <c r="M412" s="3">
         <v>1891.6</v>
       </c>
-      <c r="N412" s="8">
+      <c r="N412" s="5">
         <f t="shared" si="6"/>
         <v>1472</v>
       </c>
@@ -19155,7 +19149,7 @@
       <c r="M413" s="3">
         <v>2138.1999999999998</v>
       </c>
-      <c r="N413" s="8">
+      <c r="N413" s="5">
         <f t="shared" si="6"/>
         <v>1808</v>
       </c>
@@ -19200,12 +19194,12 @@
       <c r="M414" s="3">
         <v>2381.6999999999998</v>
       </c>
-      <c r="N414" s="8">
+      <c r="N414" s="5">
         <f t="shared" si="6"/>
         <v>2000.0000000000005</v>
       </c>
       <c r="O414" s="3"/>
-      <c r="P414" s="10"/>
+      <c r="P414" s="7"/>
     </row>
     <row r="415" spans="1:16">
       <c r="A415" s="2">
@@ -19247,7 +19241,7 @@
       <c r="M415" s="3">
         <v>2681.5</v>
       </c>
-      <c r="N415" s="8">
+      <c r="N415" s="5">
         <f t="shared" si="6"/>
         <v>2289</v>
       </c>
@@ -19292,7 +19286,7 @@
       <c r="M416" s="3">
         <v>2949.1</v>
       </c>
-      <c r="N416" s="8">
+      <c r="N416" s="5">
         <f t="shared" si="6"/>
         <v>2724</v>
       </c>
@@ -19337,7 +19331,7 @@
       <c r="M417" s="3">
         <v>0</v>
       </c>
-      <c r="N417" s="8">
+      <c r="N417" s="5">
         <f t="shared" si="6"/>
         <v>407</v>
       </c>
@@ -19382,7 +19376,7 @@
       <c r="M418" s="3">
         <v>694.5</v>
       </c>
-      <c r="N418" s="8">
+      <c r="N418" s="5">
         <f t="shared" si="6"/>
         <v>739</v>
       </c>
@@ -19427,7 +19421,7 @@
       <c r="M419" s="3">
         <v>1072.9000000000001</v>
       </c>
-      <c r="N419" s="8">
+      <c r="N419" s="5">
         <f t="shared" si="6"/>
         <v>894.99999999999989</v>
       </c>
@@ -19472,7 +19466,7 @@
       <c r="M420" s="3">
         <v>1426.3</v>
       </c>
-      <c r="N420" s="8">
+      <c r="N420" s="5">
         <f t="shared" si="6"/>
         <v>831</v>
       </c>
@@ -19517,7 +19511,7 @@
       <c r="M421" s="3">
         <v>1819.9</v>
       </c>
-      <c r="N421" s="8">
+      <c r="N421" s="5">
         <f t="shared" si="6"/>
         <v>879</v>
       </c>
@@ -19562,7 +19556,7 @@
       <c r="M422" s="3">
         <v>2219</v>
       </c>
-      <c r="N422" s="8">
+      <c r="N422" s="5">
         <f t="shared" si="6"/>
         <v>891</v>
       </c>
@@ -19607,7 +19601,7 @@
       <c r="M423" s="3">
         <v>2713.7</v>
       </c>
-      <c r="N423" s="8">
+      <c r="N423" s="5">
         <f t="shared" si="6"/>
         <v>961</v>
       </c>
@@ -19652,7 +19646,7 @@
       <c r="M424" s="3">
         <v>3223.8</v>
       </c>
-      <c r="N424" s="8">
+      <c r="N424" s="5">
         <f t="shared" si="6"/>
         <v>1196</v>
       </c>
@@ -19697,7 +19691,7 @@
       <c r="M425" s="3">
         <v>3709.2</v>
       </c>
-      <c r="N425" s="8">
+      <c r="N425" s="5">
         <f t="shared" si="6"/>
         <v>1324</v>
       </c>
@@ -19707,70 +19701,111 @@
         <v>45230</v>
       </c>
       <c r="B426" s="3">
-        <v>17405</v>
+        <v>17404.599999999999</v>
       </c>
       <c r="C426" s="3">
-        <v>47321.799999999996</v>
+        <v>47322</v>
       </c>
       <c r="D426" s="3">
-        <v>3884.8</v>
+        <v>3884.9999999999995</v>
       </c>
       <c r="E426" s="3">
-        <v>5309.4000000000005</v>
+        <v>5309</v>
       </c>
       <c r="F426" s="3">
-        <v>1341.9630903667191</v>
+        <v>1341.881535</v>
       </c>
       <c r="G426" s="3">
-        <v>1896</v>
+        <v>1896.3</v>
       </c>
       <c r="H426" s="3">
-        <v>618760000</v>
+        <v>618762000</v>
       </c>
       <c r="I426" s="3">
         <v>382922</v>
       </c>
       <c r="J426" s="3">
-        <v>3599.2</v>
+        <v>3598.9999999999995</v>
       </c>
       <c r="K426" s="3">
-        <v>0</v>
+        <v>13555.7</v>
       </c>
       <c r="L426" s="3">
-        <v>0</v>
+        <v>18098.5</v>
       </c>
       <c r="M426" s="3">
-        <v>0</v>
-      </c>
-      <c r="N426" s="8">
+        <v>4164.2</v>
+      </c>
+      <c r="N426" s="5">
         <f>E426-D426</f>
-        <v>1424.6000000000004</v>
-      </c>
-      <c r="O426" s="9"/>
+        <v>1424.0000000000005</v>
+      </c>
+      <c r="O426" s="6"/>
+    </row>
+    <row r="427" spans="1:15">
+      <c r="A427" s="2">
+        <v>45260</v>
+      </c>
+      <c r="B427" s="3">
+        <v>19125</v>
+      </c>
+      <c r="C427" s="3">
+        <v>51564.800000000003</v>
+      </c>
+      <c r="D427" s="3">
+        <v>4322.5</v>
+      </c>
+      <c r="E427" s="3">
+        <v>5817.5999999999995</v>
+      </c>
+      <c r="F427" s="3">
+        <v>0</v>
+      </c>
+      <c r="G427" s="3">
+        <v>2096</v>
+      </c>
+      <c r="H427" s="3">
+        <v>676220000</v>
+      </c>
+      <c r="I427" s="3">
+        <v>423877</v>
+      </c>
+      <c r="J427" s="3">
+        <v>4350.5999999999995</v>
+      </c>
+      <c r="K427" s="3">
+        <v>0</v>
+      </c>
+      <c r="L427" s="3">
+        <v>0</v>
+      </c>
+      <c r="M427" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="429" spans="1:15">
-      <c r="B429" s="7"/>
-      <c r="C429" s="7"/>
-      <c r="D429" s="7"/>
-      <c r="E429" s="7"/>
-      <c r="F429" s="7"/>
-      <c r="G429" s="7"/>
-      <c r="H429" s="7"/>
-      <c r="I429" s="7"/>
-      <c r="J429" s="7"/>
-      <c r="N429" s="7"/>
+      <c r="B429" s="4"/>
+      <c r="C429" s="4"/>
+      <c r="D429" s="4"/>
+      <c r="E429" s="4"/>
+      <c r="F429" s="4"/>
+      <c r="G429" s="4"/>
+      <c r="H429" s="4"/>
+      <c r="I429" s="4"/>
+      <c r="J429" s="4"/>
+      <c r="N429" s="4"/>
     </row>
     <row r="430" spans="1:15">
-      <c r="B430" s="8"/>
-      <c r="C430" s="8"/>
-      <c r="D430" s="8"/>
-      <c r="E430" s="8"/>
-      <c r="F430" s="8"/>
-      <c r="G430" s="8"/>
-      <c r="H430" s="8"/>
-      <c r="I430" s="8"/>
-      <c r="J430" s="8"/>
-      <c r="N430" s="8"/>
+      <c r="B430" s="5"/>
+      <c r="C430" s="5"/>
+      <c r="D430" s="5"/>
+      <c r="E430" s="5"/>
+      <c r="F430" s="5"/>
+      <c r="G430" s="5"/>
+      <c r="H430" s="5"/>
+      <c r="I430" s="5"/>
+      <c r="J430" s="5"/>
+      <c r="N430" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>